<commit_message>
Started implementing login stuff
</commit_message>
<xml_diff>
--- a/Docs/Suvestine.xlsx
+++ b/Docs/Suvestine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robertas\Desktop\Interaktyvios-interneto-technologijos\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041C4AF-CC46-47FE-859E-7FC5079F8896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE410F0C-9F7E-4513-B962-7B796D262721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Darbas</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Automobilio Database,Api</t>
+  </si>
+  <si>
+    <t>Login with JWT and logout</t>
+  </si>
+  <si>
+    <t>17,00-</t>
   </si>
 </sst>
 </file>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +418,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding multiple pictures works
</commit_message>
<xml_diff>
--- a/Docs/Suvestine.xlsx
+++ b/Docs/Suvestine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robertas\Desktop\Interaktyvios-interneto-technologijos\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3B80ED-C44E-4FD5-889B-22A5E02900B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505B1C90-A841-4881-A445-E6A1C22D1DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Darbas</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Paveiksleliu lentele ir prototipinis api</t>
+  </si>
+  <si>
+    <t>Paveiksleliu api taisymas ir frontendas</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C14"/>
+  <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -513,6 +516,14 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit before i mess it up
</commit_message>
<xml_diff>
--- a/Docs/Suvestine.xlsx
+++ b/Docs/Suvestine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robertas\Desktop\Interaktyvios-interneto-technologijos\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505B1C90-A841-4881-A445-E6A1C22D1DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9018EE68-5874-4F2B-8FA8-4609CFBA8087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Darbas</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Paveiksleliu api taisymas ir frontendas</t>
+  </si>
+  <si>
+    <t>Pridejau telefono numeri su ngx mask</t>
+  </si>
+  <si>
+    <t>Padariau kad isikeltu daug paveiksleliu ir isirasytu i db</t>
   </si>
 </sst>
 </file>
@@ -400,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C15"/>
+  <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -408,7 +414,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -524,6 +530,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit in case my pc burns down
</commit_message>
<xml_diff>
--- a/Docs/Suvestine.xlsx
+++ b/Docs/Suvestine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robertas\Desktop\Interaktyvios-interneto-technologijos\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BA67A2-7EBC-4B5C-B887-509A1D68974F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789C94A6-B02C-47F9-A156-AF336E4FA6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Darbas</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Skelbimu saraso redesign</t>
+  </si>
+  <si>
+    <t>Paveiksleliu api taisymas kad skelbimas rastu savo pics</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C18"/>
+  <dimension ref="B2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +560,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>